<commit_message>
Change in fom cost calculation for RES when not invested
fom costs of RES are added to total costs in output preparation file if no investment was done
</commit_message>
<xml_diff>
--- a/Spine_Projects/01_input_data/01_input_raw/Products/methane/Model_Data_Base_methane_4_InOutputs.xlsx
+++ b/Spine_Projects/01_input_data/01_input_raw/Products/methane/Model_Data_Base_methane_4_InOutputs.xlsx
@@ -474,7 +474,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -485,8 +485,7 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -940,7 +939,7 @@
   <dimension ref="A1:R17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F19" sqref="A14:F19"/>
+      <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1119,12 +1118,12 @@
       <c r="F15" s="6"/>
     </row>
     <row r="16" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A16" s="7"/>
-      <c r="B16" s="7"/>
-      <c r="C16" s="7"/>
-      <c r="D16" s="7"/>
-      <c r="E16" s="7"/>
-      <c r="F16" s="7"/>
+      <c r="A16" s="4"/>
+      <c r="B16" s="4"/>
+      <c r="C16" s="4"/>
+      <c r="D16" s="4"/>
+      <c r="E16" s="4"/>
+      <c r="F16" s="4"/>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A17" s="6"/>

</xml_diff>